<commit_message>
updated dsafnetcopy and dsafnetcopy test
</commit_message>
<xml_diff>
--- a/results/optimized_dsafnet_metrics.xlsx
+++ b/results/optimized_dsafnet_metrics.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,6 +466,11 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
+          <t>learning_rate</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
           <t>epoch_time</t>
         </is>
       </c>
@@ -475,22 +480,181 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>0.9021497220838153</v>
+        <v>0.9033397331730119</v>
       </c>
       <c r="C2" t="n">
-        <v>0.8976490282036532</v>
+        <v>0.8458161743650658</v>
       </c>
       <c r="D2" t="n">
-        <v>7.245462867021163</v>
+        <v>6.391531875526314</v>
       </c>
       <c r="E2" t="n">
-        <v>0.06097274704216913</v>
+        <v>0.1672741257265296</v>
       </c>
       <c r="F2" t="n">
-        <v>9.496172518159819</v>
+        <v>8.945469716399325</v>
       </c>
       <c r="G2" t="n">
-        <v>59.17966508865356</v>
+        <v>0.0005</v>
+      </c>
+      <c r="H2" t="n">
+        <v>71.36291837692261</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="n">
+        <v>0.8928861508789859</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.900063429837065</v>
+      </c>
+      <c r="D3" t="n">
+        <v>7.298406696147556</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.05504867505692453</v>
+      </c>
+      <c r="F3" t="n">
+        <v>9.523915326063696</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.0005</v>
+      </c>
+      <c r="H3" t="n">
+        <v>58.57611536979675</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="n">
+        <v>0.8904605047332161</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.8825040088079323</v>
+      </c>
+      <c r="D4" t="n">
+        <v>6.971020179235587</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.09011494626397053</v>
+      </c>
+      <c r="F4" t="n">
+        <v>9.345961646774244</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.0005</v>
+      </c>
+      <c r="H4" t="n">
+        <v>52.9040858745575</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0.8889403258841442</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.8606795145820689</v>
+      </c>
+      <c r="D5" t="n">
+        <v>6.685294652557366</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.1366448900075727</v>
+      </c>
+      <c r="F5" t="n">
+        <v>9.107482272116034</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.0005</v>
+      </c>
+      <c r="H5" t="n">
+        <v>53.81499409675598</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="n">
+        <v>0.8884218232122763</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.871254037527264</v>
+      </c>
+      <c r="D6" t="n">
+        <v>6.839464001744581</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.1149594803934071</v>
+      </c>
+      <c r="F6" t="n">
+        <v>9.218530078513517</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.0005</v>
+      </c>
+      <c r="H6" t="n">
+        <v>53.7888720035553</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="n">
+        <v>0.8870917813130709</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.8626975261211941</v>
+      </c>
+      <c r="D7" t="n">
+        <v>6.680427262495004</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.1324329599492154</v>
+      </c>
+      <c r="F7" t="n">
+        <v>9.1288671856053</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.00025</v>
+      </c>
+      <c r="H7" t="n">
+        <v>57.75950288772583</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="n">
+        <v>0.8867508136341025</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.8606720745404399</v>
+      </c>
+      <c r="D8" t="n">
+        <v>6.688650655584258</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.1361438733672364</v>
+      </c>
+      <c r="F8" t="n">
+        <v>9.110516361816915</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.00025</v>
+      </c>
+      <c r="H8" t="n">
+        <v>61.31318712234497</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed dsafnet full , test, copy
</commit_message>
<xml_diff>
--- a/results/optimized_dsafnet_metrics.xlsx
+++ b/results/optimized_dsafnet_metrics.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -480,25 +480,25 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>0.9033397331730119</v>
+        <v>0.9500767273996933</v>
       </c>
       <c r="C2" t="n">
-        <v>0.8458161743650658</v>
+        <v>0.884402144920482</v>
       </c>
       <c r="D2" t="n">
-        <v>6.391531875526314</v>
+        <v>7.001170153594614</v>
       </c>
       <c r="E2" t="n">
-        <v>0.1672741257265296</v>
+        <v>0.09039013543788477</v>
       </c>
       <c r="F2" t="n">
-        <v>8.945469716399325</v>
+        <v>9.346269359461671</v>
       </c>
       <c r="G2" t="n">
         <v>0.0005</v>
       </c>
       <c r="H2" t="n">
-        <v>71.36291837692261</v>
+        <v>765.5897972583771</v>
       </c>
     </row>
     <row r="3">
@@ -506,25 +506,25 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>0.8928861508789859</v>
+        <v>0.9222321805572289</v>
       </c>
       <c r="C3" t="n">
-        <v>0.900063429837065</v>
+        <v>0.8481157187647569</v>
       </c>
       <c r="D3" t="n">
-        <v>7.298406696147556</v>
+        <v>6.484466443010827</v>
       </c>
       <c r="E3" t="n">
-        <v>0.05504867505692453</v>
+        <v>0.1616189924647666</v>
       </c>
       <c r="F3" t="n">
-        <v>9.523915326063696</v>
+        <v>8.976157299524052</v>
       </c>
       <c r="G3" t="n">
         <v>0.0005</v>
       </c>
       <c r="H3" t="n">
-        <v>58.57611536979675</v>
+        <v>789.0084707736969</v>
       </c>
     </row>
     <row r="4">
@@ -532,25 +532,25 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>0.8904605047332161</v>
+        <v>0.9171926831424652</v>
       </c>
       <c r="C4" t="n">
-        <v>0.8825040088079323</v>
+        <v>0.8432353786187508</v>
       </c>
       <c r="D4" t="n">
-        <v>6.971020179235587</v>
+        <v>6.394963945628412</v>
       </c>
       <c r="E4" t="n">
-        <v>0.09011494626397053</v>
+        <v>0.1711964466690988</v>
       </c>
       <c r="F4" t="n">
-        <v>9.345961646774244</v>
+        <v>8.925033527923178</v>
       </c>
       <c r="G4" t="n">
         <v>0.0005</v>
       </c>
       <c r="H4" t="n">
-        <v>52.9040858745575</v>
+        <v>727.3990621566772</v>
       </c>
     </row>
     <row r="5">
@@ -558,25 +558,25 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>0.8889403258841442</v>
+        <v>0.9134293626604943</v>
       </c>
       <c r="C5" t="n">
-        <v>0.8606795145820689</v>
+        <v>0.8384566104319645</v>
       </c>
       <c r="D5" t="n">
-        <v>6.685294652557366</v>
+        <v>6.292914315106318</v>
       </c>
       <c r="E5" t="n">
-        <v>0.1366448900075727</v>
+        <v>0.1805897185480053</v>
       </c>
       <c r="F5" t="n">
-        <v>9.107482272116034</v>
+        <v>8.874517706497107</v>
       </c>
       <c r="G5" t="n">
         <v>0.0005</v>
       </c>
       <c r="H5" t="n">
-        <v>53.81499409675598</v>
+        <v>725.8904123306274</v>
       </c>
     </row>
     <row r="6">
@@ -584,25 +584,25 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>0.8884218232122763</v>
+        <v>0.9067369415975779</v>
       </c>
       <c r="C6" t="n">
-        <v>0.871254037527264</v>
+        <v>0.8340029422370394</v>
       </c>
       <c r="D6" t="n">
-        <v>6.839464001744581</v>
+        <v>6.105301958136987</v>
       </c>
       <c r="E6" t="n">
-        <v>0.1149594803934071</v>
+        <v>0.1883579752882517</v>
       </c>
       <c r="F6" t="n">
-        <v>9.218530078513517</v>
+        <v>8.832806471330761</v>
       </c>
       <c r="G6" t="n">
         <v>0.0005</v>
       </c>
       <c r="H6" t="n">
-        <v>53.7888720035553</v>
+        <v>726.9392278194427</v>
       </c>
     </row>
     <row r="7">
@@ -610,25 +610,25 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>0.8870917813130709</v>
+        <v>0.9023537140019808</v>
       </c>
       <c r="C7" t="n">
-        <v>0.8626975261211941</v>
+        <v>0.8361632169861343</v>
       </c>
       <c r="D7" t="n">
-        <v>6.680427262495004</v>
+        <v>6.10420607266227</v>
       </c>
       <c r="E7" t="n">
-        <v>0.1324329599492154</v>
+        <v>0.1835962688186671</v>
       </c>
       <c r="F7" t="n">
-        <v>9.1288671856053</v>
+        <v>8.858745773762456</v>
       </c>
       <c r="G7" t="n">
-        <v>0.00025</v>
+        <v>0.0005</v>
       </c>
       <c r="H7" t="n">
-        <v>57.75950288772583</v>
+        <v>725.570999622345</v>
       </c>
     </row>
     <row r="8">
@@ -636,25 +636,129 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>0.8867508136341025</v>
+        <v>0.9008317727362197</v>
       </c>
       <c r="C8" t="n">
-        <v>0.8606720745404399</v>
+        <v>0.8357795411679437</v>
       </c>
       <c r="D8" t="n">
-        <v>6.688650655584258</v>
+        <v>6.146755393129723</v>
       </c>
       <c r="E8" t="n">
-        <v>0.1361438733672364</v>
+        <v>0.1848206841904906</v>
       </c>
       <c r="F8" t="n">
-        <v>9.110516361816915</v>
+        <v>8.851871240504861</v>
       </c>
       <c r="G8" t="n">
+        <v>0.0005</v>
+      </c>
+      <c r="H8" t="n">
+        <v>719.8843920230865</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="n">
+        <v>0.8998213666912575</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.8345535596641088</v>
+      </c>
+      <c r="D9" t="n">
+        <v>6.149560542105085</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.1875039911987971</v>
+      </c>
+      <c r="F9" t="n">
+        <v>8.837241512984766</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.0005</v>
+      </c>
+      <c r="H9" t="n">
+        <v>715.9559259414673</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="n">
+        <v>0.8993305213351814</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.8349118008082622</v>
+      </c>
+      <c r="D10" t="n">
+        <v>6.16709875938085</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.1869289891373867</v>
+      </c>
+      <c r="F10" t="n">
+        <v>8.840301968379801</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0.0005</v>
+      </c>
+      <c r="H10" t="n">
+        <v>707.900096654892</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="n">
+        <v>0.8978529829713419</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.8367227257714879</v>
+      </c>
+      <c r="D11" t="n">
+        <v>6.233067504044658</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.1841422238689149</v>
+      </c>
+      <c r="F11" t="n">
+        <v>8.855089338807163</v>
+      </c>
+      <c r="G11" t="n">
         <v>0.00025</v>
       </c>
-      <c r="H8" t="n">
-        <v>61.31318712234497</v>
+      <c r="H11" t="n">
+        <v>710.7555043697357</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="n">
+        <v>0.8975820531009798</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.8365684270449631</v>
+      </c>
+      <c r="D12" t="n">
+        <v>6.231846103882567</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.1845386960953609</v>
+      </c>
+      <c r="F12" t="n">
+        <v>8.852924217278705</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0.00025</v>
+      </c>
+      <c r="H12" t="n">
+        <v>710.539449930191</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
dsafnet test updated for csv
</commit_message>
<xml_diff>
--- a/results/optimized_dsafnet_metrics.xlsx
+++ b/results/optimized_dsafnet_metrics.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -480,25 +480,25 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>0.9500767273996933</v>
+        <v>0.9473233036264742</v>
       </c>
       <c r="C2" t="n">
-        <v>0.884402144920482</v>
+        <v>0.8646585007127243</v>
       </c>
       <c r="D2" t="n">
-        <v>7.001170153594614</v>
+        <v>6.727576163278119</v>
       </c>
       <c r="E2" t="n">
-        <v>0.09039013543788477</v>
+        <v>0.1295364744106685</v>
       </c>
       <c r="F2" t="n">
-        <v>9.346269359461671</v>
+        <v>9.144571911661934</v>
       </c>
       <c r="G2" t="n">
         <v>0.0005</v>
       </c>
       <c r="H2" t="n">
-        <v>765.5897972583771</v>
+        <v>819.063134431839</v>
       </c>
     </row>
     <row r="3">
@@ -506,25 +506,25 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>0.9222321805572289</v>
+        <v>0.9207137191793482</v>
       </c>
       <c r="C3" t="n">
-        <v>0.8481157187647569</v>
+        <v>0.8452620917010886</v>
       </c>
       <c r="D3" t="n">
-        <v>6.484466443010827</v>
+        <v>6.434947238451978</v>
       </c>
       <c r="E3" t="n">
-        <v>0.1616189924647666</v>
+        <v>0.1671304550459633</v>
       </c>
       <c r="F3" t="n">
-        <v>8.976157299524052</v>
+        <v>8.946876902319923</v>
       </c>
       <c r="G3" t="n">
         <v>0.0005</v>
       </c>
       <c r="H3" t="n">
-        <v>789.0084707736969</v>
+        <v>859.3460199832916</v>
       </c>
     </row>
     <row r="4">
@@ -532,25 +532,25 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>0.9171926831424652</v>
+        <v>0.9160640711297569</v>
       </c>
       <c r="C4" t="n">
-        <v>0.8432353786187508</v>
+        <v>0.8404924650802627</v>
       </c>
       <c r="D4" t="n">
-        <v>6.394963945628412</v>
+        <v>6.339973307222476</v>
       </c>
       <c r="E4" t="n">
-        <v>0.1711964466690988</v>
+        <v>0.1764917230629811</v>
       </c>
       <c r="F4" t="n">
-        <v>8.925033527923178</v>
+        <v>8.896647279683025</v>
       </c>
       <c r="G4" t="n">
         <v>0.0005</v>
       </c>
       <c r="H4" t="n">
-        <v>727.3990621566772</v>
+        <v>767.9169588088989</v>
       </c>
     </row>
     <row r="5">
@@ -558,25 +558,25 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>0.9134293626604943</v>
+        <v>0.9109971069681119</v>
       </c>
       <c r="C5" t="n">
-        <v>0.8384566104319645</v>
+        <v>0.8342306806593546</v>
       </c>
       <c r="D5" t="n">
-        <v>6.292914315106318</v>
+        <v>6.171756828112547</v>
       </c>
       <c r="E5" t="n">
-        <v>0.1805897185480053</v>
+        <v>0.1883877462906273</v>
       </c>
       <c r="F5" t="n">
-        <v>8.874517706497107</v>
+        <v>8.832418544750757</v>
       </c>
       <c r="G5" t="n">
         <v>0.0005</v>
       </c>
       <c r="H5" t="n">
-        <v>725.8904123306274</v>
+        <v>783.0971314907074</v>
       </c>
     </row>
     <row r="6">
@@ -584,25 +584,25 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>0.9067369415975779</v>
+        <v>0.9038225912992472</v>
       </c>
       <c r="C6" t="n">
-        <v>0.8340029422370394</v>
+        <v>0.8349076636382763</v>
       </c>
       <c r="D6" t="n">
-        <v>6.105301958136987</v>
+        <v>6.081462568196883</v>
       </c>
       <c r="E6" t="n">
-        <v>0.1883579752882517</v>
+        <v>0.1860087546218191</v>
       </c>
       <c r="F6" t="n">
-        <v>8.832806471330761</v>
+        <v>8.845689188241852</v>
       </c>
       <c r="G6" t="n">
         <v>0.0005</v>
       </c>
       <c r="H6" t="n">
-        <v>726.9392278194427</v>
+        <v>783.7204332351685</v>
       </c>
     </row>
     <row r="7">
@@ -610,25 +610,25 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>0.9023537140019808</v>
+        <v>0.9014930500370167</v>
       </c>
       <c r="C7" t="n">
-        <v>0.8361632169861343</v>
+        <v>0.8352023854755122</v>
       </c>
       <c r="D7" t="n">
-        <v>6.10420607266227</v>
+        <v>6.10531429504351</v>
       </c>
       <c r="E7" t="n">
-        <v>0.1835962688186671</v>
+        <v>0.185571996476091</v>
       </c>
       <c r="F7" t="n">
-        <v>8.858745773762456</v>
+        <v>8.847938583009025</v>
       </c>
       <c r="G7" t="n">
         <v>0.0005</v>
       </c>
       <c r="H7" t="n">
-        <v>725.570999622345</v>
+        <v>764.236739397049</v>
       </c>
     </row>
     <row r="8">
@@ -636,25 +636,25 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>0.9008317727362197</v>
+        <v>0.9002834020523903</v>
       </c>
       <c r="C8" t="n">
-        <v>0.8357795411679437</v>
+        <v>0.835267150327819</v>
       </c>
       <c r="D8" t="n">
-        <v>6.146755393129723</v>
+        <v>6.154135584051019</v>
       </c>
       <c r="E8" t="n">
-        <v>0.1848206841904906</v>
+        <v>0.1859714196191194</v>
       </c>
       <c r="F8" t="n">
-        <v>8.851871240504861</v>
+        <v>8.845531478464096</v>
       </c>
       <c r="G8" t="n">
         <v>0.0005</v>
       </c>
       <c r="H8" t="n">
-        <v>719.8843920230865</v>
+        <v>739.0147221088409</v>
       </c>
     </row>
     <row r="9">
@@ -662,25 +662,25 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>0.8998213666912575</v>
+        <v>0.8993701440413977</v>
       </c>
       <c r="C9" t="n">
-        <v>0.8345535596641088</v>
+        <v>0.8343328137826296</v>
       </c>
       <c r="D9" t="n">
-        <v>6.149560542105085</v>
+        <v>6.157277530560346</v>
       </c>
       <c r="E9" t="n">
-        <v>0.1875039911987971</v>
+        <v>0.1880624090152631</v>
       </c>
       <c r="F9" t="n">
-        <v>8.837241512984766</v>
+        <v>8.834134420163808</v>
       </c>
       <c r="G9" t="n">
         <v>0.0005</v>
       </c>
       <c r="H9" t="n">
-        <v>715.9559259414673</v>
+        <v>737.6107678413391</v>
       </c>
     </row>
     <row r="10">
@@ -688,25 +688,25 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>0.8993305213351814</v>
+        <v>0.8980539490203017</v>
       </c>
       <c r="C10" t="n">
-        <v>0.8349118008082622</v>
+        <v>0.8366366549900167</v>
       </c>
       <c r="D10" t="n">
-        <v>6.16709875938085</v>
+        <v>6.233707649998536</v>
       </c>
       <c r="E10" t="n">
-        <v>0.1869289891373867</v>
+        <v>0.1842959483610671</v>
       </c>
       <c r="F10" t="n">
-        <v>8.840301968379801</v>
+        <v>8.854365372788076</v>
       </c>
       <c r="G10" t="n">
-        <v>0.0005</v>
+        <v>0.00025</v>
       </c>
       <c r="H10" t="n">
-        <v>707.900096654892</v>
+        <v>734.1522190570831</v>
       </c>
     </row>
     <row r="11">
@@ -714,51 +714,25 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>0.8978529829713419</v>
+        <v>0.8976099145384786</v>
       </c>
       <c r="C11" t="n">
-        <v>0.8367227257714879</v>
+        <v>0.8363555998985235</v>
       </c>
       <c r="D11" t="n">
-        <v>6.233067504044658</v>
+        <v>6.225617505477151</v>
       </c>
       <c r="E11" t="n">
-        <v>0.1841422238689149</v>
+        <v>0.1848572479414538</v>
       </c>
       <c r="F11" t="n">
-        <v>8.855089338807163</v>
+        <v>8.851206045221401</v>
       </c>
       <c r="G11" t="n">
         <v>0.00025</v>
       </c>
       <c r="H11" t="n">
-        <v>710.7555043697357</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>11</v>
-      </c>
-      <c r="B12" t="n">
-        <v>0.8975820531009798</v>
-      </c>
-      <c r="C12" t="n">
-        <v>0.8365684270449631</v>
-      </c>
-      <c r="D12" t="n">
-        <v>6.231846103882567</v>
-      </c>
-      <c r="E12" t="n">
-        <v>0.1845386960953609</v>
-      </c>
-      <c r="F12" t="n">
-        <v>8.852924217278705</v>
-      </c>
-      <c r="G12" t="n">
-        <v>0.00025</v>
-      </c>
-      <c r="H12" t="n">
-        <v>710.539449930191</v>
+        <v>737.5356566905975</v>
       </c>
     </row>
   </sheetData>

</xml_diff>